<commit_message>
changes before short pilot
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Megbizonyosodott róla, hogy biztosítottak a vizsgálat elvégzéséhez szükséges feltételek? Válaszát jelölje a megadott billentyűk egyikével. </t>
   </si>
   <si>
-    <t xml:space="preserve">D: Igen, körülményeim nyugodtak, az internet kapcsolat stabil, a feladatokra tudok szánni 60 percet.    F: Nem, nincs lehetőségem nyugodt körülmények között elvégezni a feladatot.</t>
+    <t xml:space="preserve">S: Igen, körülményeim nyugodtak, az internet kapcsolat stabil, a feladatokra tudok szánni 60 percet.          D: Nem, nincs lehetőségem nyugodt körülmények között elvégezni a feladatot.</t>
   </si>
   <si>
     <t xml:space="preserve">d</t>
@@ -82,10 +82,10 @@
     <t xml:space="preserve">Hány másodperce lesz a döntésre egy-egy képről?</t>
   </si>
   <si>
-    <t xml:space="preserve">D: 2mp    F: 3mp J: 4mp   K: 5mp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A helyes válasz 3 mp. </t>
+    <t xml:space="preserve">D: 2mp    F: 3mp    J: 4mp   K: 5mp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A helyes válasz 4 mp. </t>
   </si>
   <si>
     <t xml:space="preserve">Mely billenytűvel jelzi azokat a képeket, amely hasonlít egy, az első feladatban látott képhez? </t>
@@ -106,6 +106,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -189,8 +190,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fx cross bigger. some comprehension question answers changed
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Megbizonyosodott róla, hogy biztosítottak a vizsgálat elvégzéséhez szükséges feltételek? Válaszát jelölje a megadott billentyűk egyikével. </t>
   </si>
   <si>
-    <t xml:space="preserve">S: Igen, körülményeim nyugodtak, az internet kapcsolat stabil, a feladatokra tudok szánni 60 percet.          D: Nem, nincs lehetőségem nyugodt körülmények között elvégezni a feladatot.</t>
+    <t xml:space="preserve">S: Nem, nincs lehetőségem nyugodt körülmények között elvégezni a feladatot.    D: Igen, körülményeim nyugodtak, az internet kapcsolat stabil, a feladatokra tudok szánni 60 percet.</t>
   </si>
   <si>
     <t xml:space="preserve">d</t>
@@ -166,8 +166,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,7 +195,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -235,7 +239,7 @@
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="0" t="s">

</xml_diff>

<commit_message>
extra comprehension logic (repeat if incorrect answer), formatting changes
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">CorrectAnswer</t>
   </si>
   <si>
+    <t xml:space="preserve">IncorrectAnswer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InfoRepeated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mennyi időt vesz igénybe a vizsgálat? Válaszát jelölje a megadott billentyűk egyikével. </t>
   </si>
   <si>
@@ -46,6 +52,12 @@
     <t xml:space="preserve">A helyes válasz: 50-60 perc</t>
   </si>
   <si>
+    <t xml:space="preserve">Kérjük, figyelmesen olvassa végig az alábbi instrukciókat!
+A vizsgálathoz használjon asztali számítógépet vagy laptopot. A vizsgálat nem végezhető el mobil eszközön, például okostelefonon vagy táblagépen. A feladatok elvégzéséhez szüksége lesz működő billentyűzetre és stabil internet kapcsolatra. Az optimális eredmény elérése érdekében Google Chrome, Firefox vagy Safari böngésző használata javasolt. Kérjük, használja a teljes képernyő módot.
+A kísérlet teljes körű, zavartalan figyelmet igényel. A vizsgálat két feladatból áll, és elvégzése 50-60 percet vesz igénybe. Bizonyosodjon meg róla, hogy elég időt tud szánni a vizsgálatra. Ügyeljen arra, hogy telefont, vagy más eszközöket közben ne használjon, és kerülje a másokkal való interakciót.
+A vizsgálat két feladatból áll, melyek során absztrakt képeket kell kiválogatnia a megadott szempontok szerint. A feladatok alatt és a feladatok között is lesz lehetősége rövid pihenőt tartani. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Megbizonyosodott róla, hogy biztosítottak a vizsgálat elvégzéséhez szükséges feltételek? Válaszát jelölje a megadott billentyűk egyikével. </t>
   </si>
   <si>
@@ -58,6 +70,9 @@
     <t xml:space="preserve">Köszönjük!</t>
   </si>
   <si>
+    <t xml:space="preserve">Bizonyosodjon meg róla, hogy elég időt tud a vizsgálatra szánni. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Mely billentyű jelzi azokat a képeket, amelyek maradhatnak a galériában, a bemutatott helyen?</t>
   </si>
   <si>
@@ -70,6 +85,11 @@
     <t xml:space="preserve">A helyes válasz: J billentyű.</t>
   </si>
   <si>
+    <t xml:space="preserve">Az első feladat nagyjából 20 percet vesz igénybe, közben két rövid szünettel. Ügyeljen, hogy ezek a szünetek ne legyenek 2 percnél hosszabbak. 
+A 'J' billentyűvel jelölje azokat a képeket, amelyek maradhatnak a galériában, a bemutatott helyen.
+Az 'F' billentyűvel jelölje a képeket, amelyek nem maradnak kiállítva a bemutatott helyen. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Mely billentyű jelzi azokat a képeket, amelyek nem maradhatnak a bemutatott helyen?</t>
   </si>
   <si>
@@ -86,6 +106,14 @@
   </si>
   <si>
     <t xml:space="preserve">A helyes válasz 4 mp. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A döntésre 4 másodperce lesz.
+Minden képet nézzen meg figyelmesen, és minden képre adjon választ, akkor is, ha a döntés nehéz.
+A döntését így jelölje:
+Régi - F
+Hasonló - J
+Új – K</t>
   </si>
   <si>
     <t xml:space="preserve">Mely billenytűvel jelzi azokat a képeket, amely hasonlít egy, az első feladatban látott képhez? </t>
@@ -166,9 +194,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -192,10 +224,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,7 +236,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="148.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -220,99 +253,141 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>15</v>
+      <c r="E7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attention test at encoding
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -97,6 +97,27 @@
   </si>
   <si>
     <t xml:space="preserve">A helyes válasz: F billentyű</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit gondol, ebben a körben milyen arányban tudott figyelni a képekre? Kérjük, válaszoljon őszintén. Válasza a vizsgálat bejefezésével járó jutalom (kredit, ajándékutalvány) értékét nem befolyásolja.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D: 0-24%    F: 25-49%    J: 50-74%    K: 75-100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ön ennek a körnek kevesebb, mint háromnegyedében tudott a képekre figyelni.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kérjük, próbáljon meg a továbbiakban figyelni a képekre. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit gondol, ebben a körben milyen arányban tudott figyelni a képek helyére? Kérjük, válaszoljon őszintén. Válasza a vizsgálat bejefezésével járó jutalom (kredit, ajándékutalvány) értékét nem befolyásolja.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ön ebben a körnek kevesebb, mint háromnegyedében tudott a képek helyszínére figyelni.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kérjük, próbáljon meg a továbbiakban figyelni a képek helyszínére. </t>
   </si>
   <si>
     <t xml:space="preserve">Hány másodperce lesz a döntésre egy-egy képről?</t>
@@ -129,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -150,6 +171,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,17 +220,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -224,10 +258,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -236,7 +270,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="148.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -253,7 +288,7 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -273,10 +308,10 @@
       <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -284,7 +319,7 @@
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -293,14 +328,14 @@
       <c r="D3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>16</v>
       </c>
@@ -313,14 +348,14 @@
       <c r="D4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
@@ -333,61 +368,101 @@
       <c r="D5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>24</v>
+      <c r="F9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of correct answers in comprehension questions
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">D:20-30 perc    F: 50-60 perc    J: 70-80 perc</t>
   </si>
   <si>
-    <t xml:space="preserve">b</t>
+    <t xml:space="preserve">f</t>
   </si>
   <si>
     <t xml:space="preserve">A helyes válasz: 50-60 perc</t>
@@ -61,10 +61,10 @@
     <t xml:space="preserve">Megbizonyosodott róla, hogy biztosítottak a vizsgálat elvégzéséhez szükséges feltételek? Válaszát jelölje a megadott billentyűk egyikével. </t>
   </si>
   <si>
-    <t xml:space="preserve">S: Nem, nincs lehetőségem nyugodt körülmények között elvégezni a feladatot.    D: Igen, körülményeim nyugodtak, az internet kapcsolat stabil, a feladatokra tudok szánni 60 percet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d</t>
+    <t xml:space="preserve">F: Nem, nincs lehetőségem nyugodt körülmények között elvégezni a feladatot.    J: Igen, körülményeim nyugodtak, az internet kapcsolat stabil, a feladatokra tudok szánni 60 percet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
   </si>
   <si>
     <t xml:space="preserve">Köszönjük!</t>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">D billentyű    F billentyű   J billentyű    K billentyű</t>
-  </si>
-  <si>
-    <t xml:space="preserve">j</t>
   </si>
   <si>
     <t xml:space="preserve">A helyes válasz: J billentyű.</t>
@@ -93,9 +90,6 @@
     <t xml:space="preserve">Mely billentyű jelzi azokat a képeket, amelyek nem maradhatnak a bemutatott helyen?</t>
   </si>
   <si>
-    <t xml:space="preserve">f</t>
-  </si>
-  <si>
     <t xml:space="preserve">A helyes válasz: F billentyű</t>
   </si>
   <si>
@@ -105,7 +99,10 @@
     <t xml:space="preserve">D: 0-24%    F: 25-49%    J: 50-74%    K: 75-100%</t>
   </si>
   <si>
-    <t xml:space="preserve">Ön ennek a körnek kevesebb, mint háromnegyedében tudott a képekre figyelni.</t>
+    <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevesebb, mint 75%-ban tudott a képekre figyelni.</t>
   </si>
   <si>
     <t xml:space="preserve">Kérjük, próbáljon meg a továbbiakban figyelni a képekre. </t>
@@ -114,7 +111,23 @@
     <t xml:space="preserve">Mit gondol, ebben a körben milyen arányban tudott figyelni a képek helyére? Kérjük, válaszoljon őszintén. Válasza a vizsgálat bejefezésével járó jutalom (kredit, ajándékutalvány) értékét nem befolyásolja.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ön ebben a körnek kevesebb, mint háromnegyedében tudott a képek helyszínére figyelni.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Kevesebb, mint 75%-ban tudott a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> képek helyszínére figyelni.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Kérjük, próbáljon meg a továbbiakban figyelni a képek helyszínére. </t>
@@ -260,7 +273,7 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -343,126 +356,126 @@
         <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update before final test by Attila
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -290,8 +290,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
new info in repetition of encoding info
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">A helyes válasz: J billentyű.</t>
   </si>
   <si>
-    <t xml:space="preserve">Az első feladat nagyjából 20 percet vesz igénybe, közben két rövid szünettel. Ügyeljen, hogy ezek a szünetek ne legyenek 2 percnél hosszabbak. 
+    <t xml:space="preserve">Az első feladat nagyjából 25 percet vesz igénybe, közben két rövid szünettel. Ügyeljen, hogy ezek a szünetek ne legyenek 2 percnél hosszabbak. 
 A 'J' billentyűvel jelölje azokat a képeket, amelyek maradhatnak a galériában, a bemutatott helyen.
 Az 'F' billentyűvel jelölje a képeket, amelyek nem maradnak kiállítva a bemutatott helyen. </t>
   </si>
@@ -152,23 +152,7 @@
     <t xml:space="preserve">Mit gondol, a második ‘Képfelismerés’ feladatban mennyi olyan kép volt, amit nem nézett meg figyelmesen?</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Hogy érzi, lelkiismeretesen, figyelmesen oldotta meg a feladatokat? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Kérjük, válaszoljon őszintén. Válasza a vizsgálat bejefezésével járó jutalom (kredit, ajándékutalvány) értékét nem befolyásolja.</t>
-    </r>
+    <t xml:space="preserve">Hogy érzi, lelkiismeretesen, figyelmesen oldotta meg a feladatokat? Kérjük, válaszoljon őszintén. Válasza a vizsgálat bejefezésével járó jutalom (kredit, ajándékutalvány) értékét nem befolyásolja.</t>
   </si>
   <si>
     <t xml:space="preserve">D: Igen    K: Nem</t>
@@ -184,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -205,11 +189,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -290,8 +269,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -365,7 +344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="188.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>16</v>
       </c>
@@ -385,7 +364,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="188.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
instructions and response options changed for recognition
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\experiment\computer_based_tasks\terkepesz_grid\TerKepEsz_Online\stimuli_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F61867-AC14-491C-8827-7A50887D4A96}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6671A8F-81DB-44BF-90DF-7251AB753C13}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,17 +161,17 @@
     <t>A helyes válasz: F billentyű.</t>
   </si>
   <si>
+    <t xml:space="preserve">Még 2 kérdés van hátra. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Még 1 kérdés van hátra. </t>
+  </si>
+  <si>
     <t>A döntésre 4 másodperce lesz.
 Minden képet nézzen meg figyelmesen, és minden képre adjon választ, akkor is, ha a döntés nehéz.
 A döntését így jelölje:
 Régi - F
-Új – K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Még 2 kérdés van hátra. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Még 1 kérdés van hátra. </t>
+Új – J</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -701,7 +701,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
@@ -721,7 +721,7 @@
         <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -741,7 +741,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -761,7 +761,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>